<commit_message>
Enhance name parsing logic for multi-person names and suffixes
- Improved suffix extraction with more precise regex matching
- Refined multi-person name handling to better extract first and last names
- Updated test data to reflect new parsing logic
- Added more robust handling of names with shared last names
</commit_message>
<xml_diff>
--- a/normalize_names/test_data.xlsx
+++ b/normalize_names/test_data.xlsx
@@ -27,7 +27,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
     <font>
@@ -557,10 +557,14 @@
           <t>John</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jr</t>
+          <t>Smith Jr</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -577,7 +581,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lydia</t>
+          <t>Gary</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,7 +635,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Maggie</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -727,7 +731,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Maria GarciaLopez</t>
+          <t>García-López Maria</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1067,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1090,7 +1094,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">

</xml_diff>